<commit_message>
08.02.2020 Sales MC Details
</commit_message>
<xml_diff>
--- a/2020/February/All Details/06.02.2020/MC Balance Transfer Feb'2020.xlsx
+++ b/2020/February/All Details/06.02.2020/MC Balance Transfer Feb'2020.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mugdho-Corporation\2020\February\All Details\05.02.2020\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1486CA-67EC-4DDF-8942-17A97FC69401}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="598" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="598"/>
   </bookViews>
   <sheets>
     <sheet name="Oct'19 Sales+Cost+Bank+Balanch" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,12 +22,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>LENOVO</author>
   </authors>
   <commentList>
-    <comment ref="C37" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="C37" authorId="0">
       <text>
         <r>
           <rPr>
@@ -62,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="81">
   <si>
     <t>Date</t>
   </si>
@@ -298,17 +292,20 @@
     <t>A.M Tipu Boss</t>
   </si>
   <si>
-    <t>Nabila</t>
+    <t>05.02.220</t>
   </si>
   <si>
-    <t>05.02.220</t>
+    <t>06.02.2020</t>
+  </si>
+  <si>
+    <t>Picnic ZSM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1171,7 +1168,7 @@
         <xdr:cNvPr id="1317" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1183,7 +1180,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1206,14 +1203,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1273,7 +1270,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1305,27 +1302,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1357,24 +1336,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1550,19 +1511,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BI231"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="G57" sqref="G57"/>
+      <selection pane="bottomLeft" activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="20.42578125" style="11" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" style="4" customWidth="1"/>
@@ -1583,7 +1544,7 @@
     <col min="40" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" ht="19.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:61" ht="19.5">
       <c r="A1" s="148" t="s">
         <v>20</v>
       </c>
@@ -1643,7 +1604,7 @@
       <c r="BH1" s="7"/>
       <c r="BI1" s="7"/>
     </row>
-    <row r="2" spans="1:61" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:61" ht="15">
       <c r="A2" s="149" t="s">
         <v>69</v>
       </c>
@@ -1703,7 +1664,7 @@
       <c r="BH2" s="7"/>
       <c r="BI2" s="7"/>
     </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:61">
       <c r="A3" s="158" t="s">
         <v>17</v>
       </c>
@@ -1764,7 +1725,7 @@
       <c r="BH3" s="7"/>
       <c r="BI3" s="7"/>
     </row>
-    <row r="4" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:61" ht="12.6" customHeight="1">
       <c r="A4" s="146" t="s">
         <v>0</v>
       </c>
@@ -1839,7 +1800,7 @@
       <c r="BH4" s="7"/>
       <c r="BI4" s="7"/>
     </row>
-    <row r="5" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:61" ht="12.6" customHeight="1">
       <c r="A5" s="142" t="s">
         <v>70</v>
       </c>
@@ -1919,7 +1880,7 @@
       <c r="BH5" s="7"/>
       <c r="BI5" s="7"/>
     </row>
-    <row r="6" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:61" ht="12.6" customHeight="1">
       <c r="A6" s="15" t="s">
         <v>71</v>
       </c>
@@ -1999,7 +1960,7 @@
       <c r="BH6" s="7"/>
       <c r="BI6" s="7"/>
     </row>
-    <row r="7" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:61" ht="12.6" customHeight="1">
       <c r="A7" s="15" t="s">
         <v>74</v>
       </c>
@@ -2079,7 +2040,7 @@
       <c r="BH7" s="7"/>
       <c r="BI7" s="7"/>
     </row>
-    <row r="8" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:61" ht="12.6" customHeight="1">
       <c r="A8" s="15" t="s">
         <v>75</v>
       </c>
@@ -2159,7 +2120,7 @@
       <c r="BH8" s="7"/>
       <c r="BI8" s="7"/>
     </row>
-    <row r="9" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:61" ht="12" customHeight="1">
       <c r="A9" s="15" t="s">
         <v>76</v>
       </c>
@@ -2239,22 +2200,34 @@
       <c r="BH9" s="7"/>
       <c r="BI9" s="7"/>
     </row>
-    <row r="10" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+    <row r="10" spans="1:61" ht="12.6" customHeight="1">
+      <c r="A10" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="2">
+        <v>240775</v>
+      </c>
+      <c r="C10" s="2">
+        <v>285660</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1045</v>
+      </c>
       <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>286705</v>
       </c>
       <c r="F10" s="136"/>
       <c r="G10" s="19"/>
       <c r="H10" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="64"/>
-      <c r="J10" s="64"/>
+      <c r="I10" s="64">
+        <v>660</v>
+      </c>
+      <c r="J10" s="64" t="s">
+        <v>79</v>
+      </c>
       <c r="K10" s="7"/>
       <c r="L10" s="129"/>
       <c r="M10" s="129"/>
@@ -2307,7 +2280,7 @@
       <c r="BH10" s="7"/>
       <c r="BI10" s="7"/>
     </row>
-    <row r="11" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:61" ht="12.6" customHeight="1">
       <c r="A11" s="15"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2375,7 +2348,7 @@
       <c r="BH11" s="7"/>
       <c r="BI11" s="7"/>
     </row>
-    <row r="12" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:61" ht="12.6" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2443,7 +2416,7 @@
       <c r="BH12" s="7"/>
       <c r="BI12" s="7"/>
     </row>
-    <row r="13" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:61" ht="12.6" customHeight="1">
       <c r="A13" s="15"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2511,7 +2484,7 @@
       <c r="BH13" s="7"/>
       <c r="BI13" s="7"/>
     </row>
-    <row r="14" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:61" ht="12.6" customHeight="1">
       <c r="A14" s="15"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -2579,7 +2552,7 @@
       <c r="BH14" s="7"/>
       <c r="BI14" s="7"/>
     </row>
-    <row r="15" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:61" ht="12.6" customHeight="1">
       <c r="A15" s="15"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -2647,7 +2620,7 @@
       <c r="BH15" s="7"/>
       <c r="BI15" s="7"/>
     </row>
-    <row r="16" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:61" ht="12.6" customHeight="1">
       <c r="A16" s="15"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2715,7 +2688,7 @@
       <c r="BH16" s="7"/>
       <c r="BI16" s="7"/>
     </row>
-    <row r="17" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:61" ht="12.6" customHeight="1">
       <c r="A17" s="15"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2783,7 +2756,7 @@
       <c r="BH17" s="7"/>
       <c r="BI17" s="7"/>
     </row>
-    <row r="18" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:61" ht="12.6" customHeight="1">
       <c r="A18" s="15"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2851,7 +2824,7 @@
       <c r="BH18" s="7"/>
       <c r="BI18" s="7"/>
     </row>
-    <row r="19" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:61" ht="12.6" customHeight="1">
       <c r="A19" s="15"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2919,7 +2892,7 @@
       <c r="BH19" s="7"/>
       <c r="BI19" s="7"/>
     </row>
-    <row r="20" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:61" ht="12.6" customHeight="1">
       <c r="A20" s="15"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2987,7 +2960,7 @@
       <c r="BH20" s="7"/>
       <c r="BI20" s="7"/>
     </row>
-    <row r="21" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:61" ht="12.6" customHeight="1">
       <c r="A21" s="15"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -3055,7 +3028,7 @@
       <c r="BH21" s="7"/>
       <c r="BI21" s="7"/>
     </row>
-    <row r="22" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:61" ht="12.6" customHeight="1">
       <c r="A22" s="15"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -3123,7 +3096,7 @@
       <c r="BH22" s="7"/>
       <c r="BI22" s="7"/>
     </row>
-    <row r="23" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:61" ht="12.6" customHeight="1">
       <c r="A23" s="15"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -3191,7 +3164,7 @@
       <c r="BH23" s="7"/>
       <c r="BI23" s="7"/>
     </row>
-    <row r="24" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:61" ht="12.6" customHeight="1">
       <c r="A24" s="15"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -3259,7 +3232,7 @@
       <c r="BH24" s="7"/>
       <c r="BI24" s="7"/>
     </row>
-    <row r="25" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:61" ht="12.6" customHeight="1">
       <c r="A25" s="15"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -3327,7 +3300,7 @@
       <c r="BH25" s="7"/>
       <c r="BI25" s="7"/>
     </row>
-    <row r="26" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:61" ht="12.6" customHeight="1">
       <c r="A26" s="15"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -3395,7 +3368,7 @@
       <c r="BH26" s="7"/>
       <c r="BI26" s="7"/>
     </row>
-    <row r="27" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:61" ht="12.6" customHeight="1">
       <c r="A27" s="15"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -3463,7 +3436,7 @@
       <c r="BH27" s="7"/>
       <c r="BI27" s="7"/>
     </row>
-    <row r="28" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:61" ht="12.6" customHeight="1">
       <c r="A28" s="15"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -3531,7 +3504,7 @@
       <c r="BH28" s="7"/>
       <c r="BI28" s="7"/>
     </row>
-    <row r="29" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:61" ht="12.6" customHeight="1">
       <c r="A29" s="15"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -3599,7 +3572,7 @@
       <c r="BH29" s="7"/>
       <c r="BI29" s="7"/>
     </row>
-    <row r="30" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:61" ht="12.6" customHeight="1">
       <c r="A30" s="15"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -3667,7 +3640,7 @@
       <c r="BH30" s="7"/>
       <c r="BI30" s="7"/>
     </row>
-    <row r="31" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:61" ht="12.6" customHeight="1">
       <c r="A31" s="15"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -3735,7 +3708,7 @@
       <c r="BH31" s="7"/>
       <c r="BI31" s="7"/>
     </row>
-    <row r="32" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:61" ht="12.6" customHeight="1">
       <c r="A32" s="15"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -3801,29 +3774,29 @@
       <c r="BH32" s="7"/>
       <c r="BI32" s="7"/>
     </row>
-    <row r="33" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:61">
       <c r="A33" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B33" s="2">
         <f>SUM(B5:B32)</f>
-        <v>1540535</v>
+        <v>1781310</v>
       </c>
       <c r="C33" s="2">
         <f>SUM(C5:C32)</f>
-        <v>1573628</v>
+        <v>1859288</v>
       </c>
       <c r="D33" s="2">
         <f>SUM(D5:D32)</f>
-        <v>5225</v>
+        <v>6270</v>
       </c>
       <c r="E33" s="2">
         <f>SUM(E5:E32)</f>
-        <v>1578853</v>
+        <v>1865558</v>
       </c>
       <c r="F33" s="94">
         <f>B33-E33</f>
-        <v>-38318</v>
+        <v>-84248</v>
       </c>
       <c r="G33" s="114"/>
       <c r="H33" s="124"/>
@@ -3881,7 +3854,7 @@
       <c r="BH33" s="7"/>
       <c r="BI33" s="7"/>
     </row>
-    <row r="34" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:61" ht="12.6" customHeight="1">
       <c r="A34" s="8"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -3944,7 +3917,7 @@
       <c r="BH34" s="7"/>
       <c r="BI34" s="7"/>
     </row>
-    <row r="35" spans="1:61" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:61" ht="12.6" customHeight="1" thickBot="1">
       <c r="A35" s="159" t="s">
         <v>7</v>
       </c>
@@ -4009,7 +3982,7 @@
       <c r="BH35" s="7"/>
       <c r="BI35" s="7"/>
     </row>
-    <row r="36" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:61" ht="12.6" customHeight="1">
       <c r="A36" s="38" t="s">
         <v>8</v>
       </c>
@@ -4086,7 +4059,7 @@
       <c r="BH36" s="7"/>
       <c r="BI36" s="7"/>
     </row>
-    <row r="37" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:61" ht="12.6" customHeight="1">
       <c r="A37" s="12" t="s">
         <v>27</v>
       </c>
@@ -4157,7 +4130,7 @@
       <c r="BH37" s="7"/>
       <c r="BI37" s="7"/>
     </row>
-    <row r="38" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:61" ht="12.6" customHeight="1">
       <c r="A38" s="12" t="s">
         <v>55</v>
       </c>
@@ -4228,7 +4201,7 @@
       <c r="BH38" s="7"/>
       <c r="BI38" s="7"/>
     </row>
-    <row r="39" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:61" ht="12.6" customHeight="1">
       <c r="A39" s="12" t="s">
         <v>47</v>
       </c>
@@ -4299,7 +4272,7 @@
       <c r="BH39" s="7"/>
       <c r="BI39" s="7"/>
     </row>
-    <row r="40" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:61" ht="12.6" customHeight="1">
       <c r="A40" s="12" t="s">
         <v>38</v>
       </c>
@@ -4370,7 +4343,7 @@
       <c r="BH40" s="7"/>
       <c r="BI40" s="7"/>
     </row>
-    <row r="41" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:61" ht="12.6" customHeight="1">
       <c r="A41" s="40" t="s">
         <v>72</v>
       </c>
@@ -4441,7 +4414,7 @@
       <c r="BH41" s="7"/>
       <c r="BI41" s="7"/>
     </row>
-    <row r="42" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:61" ht="12.6" customHeight="1">
       <c r="A42" s="47" t="s">
         <v>31</v>
       </c>
@@ -4511,7 +4484,7 @@
       <c r="BH42" s="7"/>
       <c r="BI42" s="7"/>
     </row>
-    <row r="43" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:61" ht="12.6" customHeight="1">
       <c r="A43" s="12" t="s">
         <v>57</v>
       </c>
@@ -4584,11 +4557,11 @@
       <c r="BH43" s="7"/>
       <c r="BI43" s="7"/>
     </row>
-    <row r="44" spans="1:61" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:61" ht="12.6" customHeight="1" thickBot="1">
       <c r="A44" s="73"/>
       <c r="B44" s="74"/>
       <c r="C44" s="75">
-        <v>8053</v>
+        <v>1473</v>
       </c>
       <c r="D44" s="76"/>
       <c r="E44" s="3"/>
@@ -4647,7 +4620,7 @@
       <c r="BH44" s="7"/>
       <c r="BI44" s="7"/>
     </row>
-    <row r="45" spans="1:61" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:61" ht="12" customHeight="1" thickTop="1" thickBot="1">
       <c r="A45" s="69"/>
       <c r="B45" s="70"/>
       <c r="C45" s="71"/>
@@ -4708,7 +4681,7 @@
       <c r="BH45" s="7"/>
       <c r="BI45" s="7"/>
     </row>
-    <row r="46" spans="1:61" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:61" ht="12" customHeight="1" thickTop="1">
       <c r="A46" s="101" t="s">
         <v>22</v>
       </c>
@@ -4775,7 +4748,7 @@
       <c r="BH46" s="7"/>
       <c r="BI46" s="7"/>
     </row>
-    <row r="47" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:61" ht="12.75" customHeight="1">
       <c r="A47" s="104" t="s">
         <v>23</v>
       </c>
@@ -4842,7 +4815,7 @@
       <c r="BH47" s="7"/>
       <c r="BI47" s="7"/>
     </row>
-    <row r="48" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:61" ht="12" customHeight="1">
       <c r="A48" s="105" t="s">
         <v>29</v>
       </c>
@@ -4908,7 +4881,7 @@
       <c r="BH48" s="7"/>
       <c r="BI48" s="7"/>
     </row>
-    <row r="49" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:61">
       <c r="A49" s="100"/>
       <c r="B49" s="43"/>
       <c r="C49" s="98"/>
@@ -4969,16 +4942,16 @@
       <c r="BH49" s="7"/>
       <c r="BI49" s="7"/>
     </row>
-    <row r="50" spans="1:61" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:61" ht="11.25" customHeight="1">
       <c r="A50" s="105" t="s">
         <v>24</v>
       </c>
       <c r="B50" s="43"/>
       <c r="C50" s="98">
-        <v>99300</v>
+        <v>98090</v>
       </c>
       <c r="D50" s="102" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="12"/>
@@ -5036,13 +5009,13 @@
       <c r="BH50" s="7"/>
       <c r="BI50" s="7"/>
     </row>
-    <row r="51" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:61" ht="12" customHeight="1">
       <c r="A51" s="105" t="s">
         <v>28</v>
       </c>
       <c r="B51" s="43"/>
       <c r="C51" s="98">
-        <v>568055</v>
+        <v>518055</v>
       </c>
       <c r="D51" s="99" t="s">
         <v>76</v>
@@ -5105,16 +5078,16 @@
       <c r="BH51" s="7"/>
       <c r="BI51" s="7"/>
     </row>
-    <row r="52" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:61" ht="12" customHeight="1">
       <c r="A52" s="105" t="s">
         <v>33</v>
       </c>
       <c r="B52" s="43"/>
       <c r="C52" s="98">
-        <v>194283</v>
+        <v>197958</v>
       </c>
       <c r="D52" s="102" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="12"/>
@@ -5174,16 +5147,16 @@
       <c r="BH52" s="7"/>
       <c r="BI52" s="7"/>
     </row>
-    <row r="53" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:61" ht="12" customHeight="1">
       <c r="A53" s="100" t="s">
         <v>34</v>
       </c>
       <c r="B53" s="97"/>
       <c r="C53" s="106">
-        <v>43000</v>
+        <v>33000</v>
       </c>
       <c r="D53" s="99" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="64"/>
@@ -5243,7 +5216,7 @@
       <c r="BH53" s="7"/>
       <c r="BI53" s="7"/>
     </row>
-    <row r="54" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:61" ht="12" customHeight="1">
       <c r="A54" s="100" t="s">
         <v>35</v>
       </c>
@@ -5312,7 +5285,7 @@
       <c r="BH54" s="7"/>
       <c r="BI54" s="7"/>
     </row>
-    <row r="55" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:61" ht="12" customHeight="1">
       <c r="A55" s="100"/>
       <c r="B55" s="44"/>
       <c r="C55" s="98"/>
@@ -5377,7 +5350,7 @@
       <c r="BH55" s="7"/>
       <c r="BI55" s="7"/>
     </row>
-    <row r="56" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:61" ht="12" customHeight="1">
       <c r="A56" s="100" t="s">
         <v>41</v>
       </c>
@@ -5446,7 +5419,7 @@
       <c r="BH56" s="7"/>
       <c r="BI56" s="7"/>
     </row>
-    <row r="57" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:61" ht="12" customHeight="1">
       <c r="A57" s="100"/>
       <c r="B57" s="43"/>
       <c r="C57" s="98"/>
@@ -5509,11 +5482,17 @@
       <c r="BH57" s="7"/>
       <c r="BI57" s="7"/>
     </row>
-    <row r="58" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="100"/>
+    <row r="58" spans="1:61" ht="12" customHeight="1">
+      <c r="A58" s="100" t="s">
+        <v>80</v>
+      </c>
       <c r="B58" s="43"/>
-      <c r="C58" s="98"/>
-      <c r="D58" s="107"/>
+      <c r="C58" s="98">
+        <v>3000</v>
+      </c>
+      <c r="D58" s="107" t="s">
+        <v>79</v>
+      </c>
       <c r="E58" s="3"/>
       <c r="F58" s="64"/>
       <c r="G58" s="12"/>
@@ -5572,7 +5551,7 @@
       <c r="BH58" s="7"/>
       <c r="BI58" s="7"/>
     </row>
-    <row r="59" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:61" ht="12" customHeight="1">
       <c r="A59" s="100" t="s">
         <v>65</v>
       </c>
@@ -5581,7 +5560,7 @@
         <v>7500</v>
       </c>
       <c r="D59" s="107" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="43"/>
@@ -5641,16 +5620,16 @@
       <c r="BH59" s="7"/>
       <c r="BI59" s="7"/>
     </row>
-    <row r="60" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:61" ht="12" customHeight="1">
       <c r="A60" s="105" t="s">
         <v>62</v>
       </c>
       <c r="B60" s="43"/>
       <c r="C60" s="98">
-        <v>89180</v>
+        <v>104635</v>
       </c>
       <c r="D60" s="99" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="43"/>
@@ -5710,7 +5689,7 @@
       <c r="BH60" s="7"/>
       <c r="BI60" s="7"/>
     </row>
-    <row r="61" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:61" ht="12" customHeight="1">
       <c r="A61" s="100" t="s">
         <v>59</v>
       </c>
@@ -5779,7 +5758,7 @@
       <c r="BH61" s="7"/>
       <c r="BI61" s="7"/>
     </row>
-    <row r="62" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:61" ht="12.75" customHeight="1">
       <c r="A62" s="100"/>
       <c r="B62" s="43"/>
       <c r="C62" s="98"/>
@@ -5850,7 +5829,7 @@
       <c r="BH62" s="7"/>
       <c r="BI62" s="7"/>
     </row>
-    <row r="63" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:61" ht="12.75" customHeight="1">
       <c r="A63" s="100" t="s">
         <v>60</v>
       </c>
@@ -5922,7 +5901,7 @@
       <c r="BH63" s="7"/>
       <c r="BI63" s="7"/>
     </row>
-    <row r="64" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:61" ht="12.75" customHeight="1">
       <c r="A64" s="105" t="s">
         <v>77</v>
       </c>
@@ -6002,17 +5981,11 @@
       <c r="BH64" s="7"/>
       <c r="BI64" s="7"/>
     </row>
-    <row r="65" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="100" t="s">
-        <v>78</v>
-      </c>
+    <row r="65" spans="1:61" ht="12.75" customHeight="1">
+      <c r="A65" s="100"/>
       <c r="B65" s="43"/>
-      <c r="C65" s="98">
-        <v>270</v>
-      </c>
-      <c r="D65" s="99" t="s">
-        <v>76</v>
-      </c>
+      <c r="C65" s="98"/>
+      <c r="D65" s="99"/>
       <c r="E65" s="3"/>
       <c r="F65" s="24"/>
       <c r="G65" s="13" t="s">
@@ -6084,7 +6057,7 @@
       <c r="BH65" s="7"/>
       <c r="BI65" s="7"/>
     </row>
-    <row r="66" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:61" ht="12.75" customHeight="1">
       <c r="A66" s="100"/>
       <c r="B66" s="43"/>
       <c r="C66" s="98"/>
@@ -6160,7 +6133,7 @@
       <c r="BH66" s="7"/>
       <c r="BI66" s="7"/>
     </row>
-    <row r="67" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:61" ht="12.75" customHeight="1">
       <c r="A67" s="105"/>
       <c r="B67" s="43"/>
       <c r="C67" s="98"/>
@@ -6236,7 +6209,7 @@
       <c r="BH67" s="7"/>
       <c r="BI67" s="7"/>
     </row>
-    <row r="68" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:61" ht="12.75" customHeight="1">
       <c r="A68" s="105"/>
       <c r="B68" s="43"/>
       <c r="C68" s="98"/>
@@ -6310,7 +6283,7 @@
       <c r="BH68" s="7"/>
       <c r="BI68" s="7"/>
     </row>
-    <row r="69" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:61" ht="12.75" customHeight="1">
       <c r="A69" s="100"/>
       <c r="B69" s="43"/>
       <c r="C69" s="98"/>
@@ -6386,7 +6359,7 @@
       <c r="BH69" s="7"/>
       <c r="BI69" s="7"/>
     </row>
-    <row r="70" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:61" ht="12.75" customHeight="1">
       <c r="A70" s="100"/>
       <c r="B70" s="43"/>
       <c r="C70" s="98"/>
@@ -6460,7 +6433,7 @@
       <c r="BH70" s="7"/>
       <c r="BI70" s="7"/>
     </row>
-    <row r="71" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:61" ht="12.75" customHeight="1">
       <c r="A71" s="105"/>
       <c r="B71" s="43"/>
       <c r="C71" s="98"/>
@@ -6532,7 +6505,7 @@
       <c r="BH71" s="7"/>
       <c r="BI71" s="7"/>
     </row>
-    <row r="72" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:61" ht="12.75" customHeight="1">
       <c r="A72" s="100"/>
       <c r="B72" s="43"/>
       <c r="C72" s="98"/>
@@ -6600,7 +6573,7 @@
       <c r="BH72" s="7"/>
       <c r="BI72" s="7"/>
     </row>
-    <row r="73" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:61" ht="12.75" customHeight="1">
       <c r="A73" s="100"/>
       <c r="B73" s="43"/>
       <c r="C73" s="98"/>
@@ -6674,7 +6647,7 @@
       <c r="BH73" s="7"/>
       <c r="BI73" s="7"/>
     </row>
-    <row r="74" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:61" ht="12.75" customHeight="1">
       <c r="A74" s="100"/>
       <c r="B74" s="43"/>
       <c r="C74" s="98"/>
@@ -6748,7 +6721,7 @@
       <c r="BH74" s="7"/>
       <c r="BI74" s="7"/>
     </row>
-    <row r="75" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:61" ht="12.75" customHeight="1">
       <c r="A75" s="100"/>
       <c r="B75" s="43"/>
       <c r="C75" s="98"/>
@@ -6822,7 +6795,7 @@
       <c r="BH75" s="7"/>
       <c r="BI75" s="7"/>
     </row>
-    <row r="76" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:61" ht="12.75" customHeight="1">
       <c r="A76" s="100"/>
       <c r="B76" s="43"/>
       <c r="C76" s="98"/>
@@ -6890,7 +6863,7 @@
       <c r="BH76" s="7"/>
       <c r="BI76" s="7"/>
     </row>
-    <row r="77" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:61" ht="12.75" customHeight="1">
       <c r="A77" s="105"/>
       <c r="B77" s="43"/>
       <c r="C77" s="98"/>
@@ -6964,7 +6937,7 @@
       <c r="BH77" s="7"/>
       <c r="BI77" s="7"/>
     </row>
-    <row r="78" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:61" ht="12.75" customHeight="1">
       <c r="A78" s="100"/>
       <c r="B78" s="43"/>
       <c r="C78" s="98"/>
@@ -7038,7 +7011,7 @@
       <c r="BH78" s="7"/>
       <c r="BI78" s="7"/>
     </row>
-    <row r="79" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:61" ht="12.75" customHeight="1">
       <c r="A79" s="100"/>
       <c r="B79" s="43"/>
       <c r="C79" s="98"/>
@@ -7112,7 +7085,7 @@
       <c r="BH79" s="7"/>
       <c r="BI79" s="7"/>
     </row>
-    <row r="80" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:61" ht="12.75" customHeight="1">
       <c r="A80" s="100"/>
       <c r="B80" s="43"/>
       <c r="C80" s="98"/>
@@ -7186,7 +7159,7 @@
       <c r="BH80" s="7"/>
       <c r="BI80" s="7"/>
     </row>
-    <row r="81" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:61" ht="12.75" customHeight="1">
       <c r="A81" s="100"/>
       <c r="B81" s="43"/>
       <c r="C81" s="98"/>
@@ -7260,7 +7233,7 @@
       <c r="BH81" s="7"/>
       <c r="BI81" s="7"/>
     </row>
-    <row r="82" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:61" ht="12.75" customHeight="1">
       <c r="A82" s="100"/>
       <c r="B82" s="43"/>
       <c r="C82" s="98"/>
@@ -7328,7 +7301,7 @@
       <c r="BH82" s="7"/>
       <c r="BI82" s="7"/>
     </row>
-    <row r="83" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:61" ht="12.75" customHeight="1">
       <c r="A83" s="105"/>
       <c r="B83" s="99"/>
       <c r="C83" s="98"/>
@@ -7402,7 +7375,7 @@
       <c r="BH83" s="7"/>
       <c r="BI83" s="7"/>
     </row>
-    <row r="84" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:61" ht="12.75" customHeight="1">
       <c r="A84" s="100"/>
       <c r="B84" s="43"/>
       <c r="C84" s="98"/>
@@ -7470,7 +7443,7 @@
       <c r="BH84" s="7"/>
       <c r="BI84" s="7"/>
     </row>
-    <row r="85" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:61" ht="12.75" customHeight="1">
       <c r="A85" s="100"/>
       <c r="B85" s="43"/>
       <c r="C85" s="98"/>
@@ -7542,7 +7515,7 @@
       <c r="BH85" s="7"/>
       <c r="BI85" s="7"/>
     </row>
-    <row r="86" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:61" ht="12.75" customHeight="1">
       <c r="A86" s="100"/>
       <c r="B86" s="43"/>
       <c r="C86" s="98"/>
@@ -7614,7 +7587,7 @@
       <c r="BH86" s="7"/>
       <c r="BI86" s="7"/>
     </row>
-    <row r="87" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:61" ht="12.75" customHeight="1">
       <c r="A87" s="100"/>
       <c r="B87" s="43"/>
       <c r="C87" s="98"/>
@@ -7686,7 +7659,7 @@
       <c r="BH87" s="7"/>
       <c r="BI87" s="7"/>
     </row>
-    <row r="88" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:61" ht="12.75" customHeight="1">
       <c r="A88" s="105"/>
       <c r="B88" s="43"/>
       <c r="C88" s="98"/>
@@ -7758,7 +7731,7 @@
       <c r="BH88" s="7"/>
       <c r="BI88" s="7"/>
     </row>
-    <row r="89" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:61" ht="12.75" customHeight="1">
       <c r="A89" s="100"/>
       <c r="B89" s="43"/>
       <c r="C89" s="98"/>
@@ -7824,7 +7797,7 @@
       <c r="BH89" s="7"/>
       <c r="BI89" s="7"/>
     </row>
-    <row r="90" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:61" ht="12.6" customHeight="1">
       <c r="A90" s="100"/>
       <c r="B90" s="43"/>
       <c r="C90" s="98"/>
@@ -7896,7 +7869,7 @@
       <c r="BH90" s="7"/>
       <c r="BI90" s="7"/>
     </row>
-    <row r="91" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:61" ht="12.75" customHeight="1">
       <c r="A91" s="100"/>
       <c r="B91" s="108"/>
       <c r="C91" s="106"/>
@@ -7970,7 +7943,7 @@
       <c r="BH91" s="7"/>
       <c r="BI91" s="7"/>
     </row>
-    <row r="92" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:61">
       <c r="A92" s="100"/>
       <c r="B92" s="97"/>
       <c r="C92" s="98"/>
@@ -8041,7 +8014,7 @@
       <c r="BH92" s="7"/>
       <c r="BI92" s="7"/>
     </row>
-    <row r="93" spans="1:61" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:61" ht="14.25" customHeight="1">
       <c r="A93" s="100"/>
       <c r="B93" s="108"/>
       <c r="C93" s="98"/>
@@ -8106,7 +8079,7 @@
       <c r="BH93" s="7"/>
       <c r="BI93" s="7"/>
     </row>
-    <row r="94" spans="1:61" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:61" ht="14.25" customHeight="1">
       <c r="A94" s="105"/>
       <c r="B94" s="99"/>
       <c r="C94" s="98"/>
@@ -8179,7 +8152,7 @@
       <c r="BH94" s="7"/>
       <c r="BI94" s="7"/>
     </row>
-    <row r="95" spans="1:61" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:61" ht="14.25" customHeight="1">
       <c r="A95" s="100"/>
       <c r="B95" s="97"/>
       <c r="C95" s="98"/>
@@ -8252,7 +8225,7 @@
       <c r="BH95" s="7"/>
       <c r="BI95" s="7"/>
     </row>
-    <row r="96" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:61">
       <c r="A96" s="118" t="s">
         <v>43</v>
       </c>
@@ -8323,7 +8296,7 @@
       <c r="BH96" s="7"/>
       <c r="BI96" s="7"/>
     </row>
-    <row r="97" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:61">
       <c r="A97" s="118" t="s">
         <v>54</v>
       </c>
@@ -8394,14 +8367,14 @@
       <c r="BH97" s="7"/>
       <c r="BI97" s="7"/>
     </row>
-    <row r="98" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:61">
       <c r="A98" s="153" t="s">
         <v>14</v>
       </c>
       <c r="B98" s="154"/>
       <c r="C98" s="45">
         <f>SUM(C37:C97)</f>
-        <v>1863655</v>
+        <v>1817725</v>
       </c>
       <c r="D98" s="41"/>
       <c r="F98" s="23"/>
@@ -8464,7 +8437,7 @@
       <c r="BH98" s="7"/>
       <c r="BI98" s="7"/>
     </row>
-    <row r="99" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:61">
       <c r="A99" s="36"/>
       <c r="B99" s="37"/>
       <c r="C99" s="46"/>
@@ -8529,14 +8502,14 @@
       <c r="BH99" s="7"/>
       <c r="BI99" s="7"/>
     </row>
-    <row r="100" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:61">
       <c r="A100" s="151" t="s">
         <v>16</v>
       </c>
       <c r="B100" s="152"/>
       <c r="C100" s="42">
         <f>C98+L121</f>
-        <v>1863655</v>
+        <v>1817725</v>
       </c>
       <c r="D100" s="26"/>
       <c r="F100" s="24"/>
@@ -8599,7 +8572,7 @@
       <c r="BH100" s="7"/>
       <c r="BI100" s="7"/>
     </row>
-    <row r="101" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:61">
       <c r="A101" s="59"/>
       <c r="B101" s="7"/>
       <c r="C101" s="60"/>
@@ -8664,7 +8637,7 @@
       <c r="BH101" s="7"/>
       <c r="BI101" s="7"/>
     </row>
-    <row r="102" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:61">
       <c r="A102" s="59"/>
       <c r="B102" s="7"/>
       <c r="D102" s="60"/>
@@ -8728,7 +8701,7 @@
       <c r="BH102" s="7"/>
       <c r="BI102" s="7"/>
     </row>
-    <row r="103" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:61">
       <c r="A103" s="61"/>
       <c r="B103" s="61"/>
       <c r="C103" s="60"/>
@@ -8793,7 +8766,7 @@
       <c r="BH103" s="7"/>
       <c r="BI103" s="7"/>
     </row>
-    <row r="104" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:61">
       <c r="C104" s="33"/>
       <c r="F104" s="24"/>
       <c r="G104" s="13"/>
@@ -8855,7 +8828,7 @@
       <c r="BH104" s="7"/>
       <c r="BI104" s="7"/>
     </row>
-    <row r="105" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:61">
       <c r="A105" s="54"/>
       <c r="B105" s="55"/>
       <c r="C105" s="56"/>
@@ -8920,7 +8893,7 @@
       <c r="BH105" s="7"/>
       <c r="BI105" s="7"/>
     </row>
-    <row r="106" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:61">
       <c r="A106" s="54"/>
       <c r="B106" s="55"/>
       <c r="C106" s="56"/>
@@ -8985,7 +8958,7 @@
       <c r="BH106" s="7"/>
       <c r="BI106" s="7"/>
     </row>
-    <row r="107" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:61">
       <c r="A107" s="55"/>
       <c r="B107" s="58"/>
       <c r="C107" s="56"/>
@@ -9050,7 +9023,7 @@
       <c r="BH107" s="7"/>
       <c r="BI107" s="7"/>
     </row>
-    <row r="108" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:61">
       <c r="A108" s="54"/>
       <c r="B108" s="55"/>
       <c r="C108" s="56"/>
@@ -9115,7 +9088,7 @@
       <c r="BH108" s="7"/>
       <c r="BI108" s="7"/>
     </row>
-    <row r="109" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:61">
       <c r="A109" s="50"/>
       <c r="B109" s="51"/>
       <c r="C109" s="52"/>
@@ -9180,7 +9153,7 @@
       <c r="BH109" s="7"/>
       <c r="BI109" s="7"/>
     </row>
-    <row r="110" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:61">
       <c r="A110" s="50"/>
       <c r="B110" s="51"/>
       <c r="C110" s="52"/>
@@ -9245,7 +9218,7 @@
       <c r="BH110" s="7"/>
       <c r="BI110" s="7"/>
     </row>
-    <row r="111" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:61">
       <c r="A111" s="50"/>
       <c r="B111" s="51"/>
       <c r="C111" s="52"/>
@@ -9310,7 +9283,7 @@
       <c r="BH111" s="7"/>
       <c r="BI111" s="7"/>
     </row>
-    <row r="112" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:61">
       <c r="C112" s="33"/>
       <c r="F112" s="23"/>
       <c r="G112" s="13"/>
@@ -9372,7 +9345,7 @@
       <c r="BH112" s="7"/>
       <c r="BI112" s="7"/>
     </row>
-    <row r="113" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:61">
       <c r="C113" s="33"/>
       <c r="F113" s="23"/>
       <c r="G113" s="13"/>
@@ -9434,7 +9407,7 @@
       <c r="BH113" s="7"/>
       <c r="BI113" s="7"/>
     </row>
-    <row r="114" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:61">
       <c r="F114" s="14"/>
       <c r="G114" s="13"/>
       <c r="H114" s="13"/>
@@ -9495,7 +9468,7 @@
       <c r="BH114" s="7"/>
       <c r="BI114" s="7"/>
     </row>
-    <row r="115" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:61">
       <c r="F115" s="14"/>
       <c r="G115" s="13"/>
       <c r="H115" s="13"/>
@@ -9556,7 +9529,7 @@
       <c r="BH115" s="7"/>
       <c r="BI115" s="7"/>
     </row>
-    <row r="116" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:61">
       <c r="F116" s="14"/>
       <c r="G116" s="13"/>
       <c r="H116" s="13"/>
@@ -9617,7 +9590,7 @@
       <c r="BH116" s="7"/>
       <c r="BI116" s="7"/>
     </row>
-    <row r="117" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:61">
       <c r="F117" s="14"/>
       <c r="G117" s="13"/>
       <c r="H117" s="13"/>
@@ -9678,7 +9651,7 @@
       <c r="BH117" s="7"/>
       <c r="BI117" s="7"/>
     </row>
-    <row r="118" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:61">
       <c r="F118" s="14"/>
       <c r="G118" s="13"/>
       <c r="H118" s="13"/>
@@ -9739,7 +9712,7 @@
       <c r="BH118" s="7"/>
       <c r="BI118" s="7"/>
     </row>
-    <row r="119" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:61">
       <c r="A119" s="9"/>
       <c r="B119" s="7"/>
       <c r="C119" s="7"/>
@@ -9805,7 +9778,7 @@
       <c r="BH119" s="7"/>
       <c r="BI119" s="7"/>
     </row>
-    <row r="120" spans="1:61" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:61" ht="13.5" thickBot="1">
       <c r="A120" s="9"/>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
@@ -9871,7 +9844,7 @@
       <c r="BH120" s="7"/>
       <c r="BI120" s="7"/>
     </row>
-    <row r="121" spans="1:61" s="5" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:61" s="5" customFormat="1" ht="13.5" thickBot="1">
       <c r="A121" s="9"/>
       <c r="B121" s="7"/>
       <c r="C121" s="7"/>
@@ -9943,7 +9916,7 @@
       <c r="BH121" s="7"/>
       <c r="BI121" s="7"/>
     </row>
-    <row r="122" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:61">
       <c r="A122" s="9"/>
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
@@ -10006,7 +9979,7 @@
       <c r="BH122" s="7"/>
       <c r="BI122" s="7"/>
     </row>
-    <row r="123" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:61">
       <c r="A123" s="9"/>
       <c r="B123" s="7"/>
       <c r="C123" s="7"/>
@@ -10032,7 +10005,7 @@
       <c r="W123" s="7"/>
       <c r="X123" s="7"/>
     </row>
-    <row r="124" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:61">
       <c r="F124" s="7"/>
       <c r="G124" s="7"/>
       <c r="H124" s="7"/>
@@ -10053,7 +10026,7 @@
       <c r="W124" s="7"/>
       <c r="X124" s="7"/>
     </row>
-    <row r="125" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:61">
       <c r="F125" s="7"/>
       <c r="G125" s="7"/>
       <c r="H125" s="7"/>
@@ -10074,7 +10047,7 @@
       <c r="W125" s="7"/>
       <c r="X125" s="7"/>
     </row>
-    <row r="126" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:61">
       <c r="F126" s="7"/>
       <c r="G126" s="7"/>
       <c r="H126" s="7"/>
@@ -10095,7 +10068,7 @@
       <c r="W126" s="7"/>
       <c r="X126" s="7"/>
     </row>
-    <row r="127" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:61">
       <c r="F127" s="7"/>
       <c r="G127" s="7"/>
       <c r="H127" s="7"/>
@@ -10116,7 +10089,7 @@
       <c r="W127" s="7"/>
       <c r="X127" s="7"/>
     </row>
-    <row r="128" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:61">
       <c r="F128" s="7"/>
       <c r="G128" s="7"/>
       <c r="H128" s="7"/>
@@ -10137,7 +10110,7 @@
       <c r="W128" s="7"/>
       <c r="X128" s="7"/>
     </row>
-    <row r="129" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="129" spans="6:24">
       <c r="F129" s="7"/>
       <c r="G129" s="7"/>
       <c r="H129" s="7"/>
@@ -10158,7 +10131,7 @@
       <c r="W129" s="7"/>
       <c r="X129" s="7"/>
     </row>
-    <row r="130" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="130" spans="6:24">
       <c r="F130" s="7"/>
       <c r="G130" s="7"/>
       <c r="H130" s="7"/>
@@ -10176,7 +10149,7 @@
       <c r="T130" s="7"/>
       <c r="U130" s="7"/>
     </row>
-    <row r="131" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="131" spans="6:24">
       <c r="F131" s="7"/>
       <c r="G131" s="7"/>
       <c r="H131" s="7"/>
@@ -10194,7 +10167,7 @@
       <c r="T131" s="7"/>
       <c r="U131" s="7"/>
     </row>
-    <row r="132" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="132" spans="6:24">
       <c r="F132" s="7"/>
       <c r="G132" s="7"/>
       <c r="H132" s="7"/>
@@ -10212,7 +10185,7 @@
       <c r="T132" s="7"/>
       <c r="U132" s="7"/>
     </row>
-    <row r="133" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="133" spans="6:24">
       <c r="F133" s="7"/>
       <c r="G133" s="7"/>
       <c r="H133" s="7"/>
@@ -10230,7 +10203,7 @@
       <c r="T133" s="7"/>
       <c r="U133" s="7"/>
     </row>
-    <row r="134" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="134" spans="6:24">
       <c r="F134" s="7"/>
       <c r="G134" s="7"/>
       <c r="H134" s="7"/>
@@ -10248,7 +10221,7 @@
       <c r="T134" s="7"/>
       <c r="U134" s="7"/>
     </row>
-    <row r="135" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="135" spans="6:24">
       <c r="F135" s="7"/>
       <c r="G135" s="7"/>
       <c r="H135" s="7"/>
@@ -10266,7 +10239,7 @@
       <c r="T135" s="7"/>
       <c r="U135" s="7"/>
     </row>
-    <row r="136" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="136" spans="6:24">
       <c r="F136" s="7"/>
       <c r="G136" s="7"/>
       <c r="H136" s="7"/>
@@ -10284,7 +10257,7 @@
       <c r="T136" s="7"/>
       <c r="U136" s="7"/>
     </row>
-    <row r="137" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="137" spans="6:24">
       <c r="F137" s="7"/>
       <c r="G137" s="7"/>
       <c r="H137" s="7"/>
@@ -10302,7 +10275,7 @@
       <c r="T137" s="7"/>
       <c r="U137" s="7"/>
     </row>
-    <row r="138" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="138" spans="6:24">
       <c r="F138" s="7"/>
       <c r="G138" s="7"/>
       <c r="H138" s="7"/>
@@ -10320,119 +10293,119 @@
       <c r="T138" s="7"/>
       <c r="U138" s="7"/>
     </row>
-    <row r="139" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="139" spans="6:24">
       <c r="F139" s="7"/>
       <c r="G139" s="7"/>
       <c r="H139" s="7"/>
       <c r="I139" s="19"/>
       <c r="J139" s="19"/>
     </row>
-    <row r="140" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="140" spans="6:24">
       <c r="F140" s="7"/>
       <c r="G140" s="7"/>
       <c r="H140" s="7"/>
       <c r="I140" s="19"/>
       <c r="J140" s="19"/>
     </row>
-    <row r="141" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="141" spans="6:24">
       <c r="F141" s="7"/>
       <c r="G141" s="7"/>
       <c r="H141" s="7"/>
       <c r="I141" s="19"/>
       <c r="J141" s="19"/>
     </row>
-    <row r="142" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="142" spans="6:24">
       <c r="F142" s="7"/>
       <c r="G142" s="7"/>
       <c r="H142" s="7"/>
       <c r="I142" s="19"/>
       <c r="J142" s="19"/>
     </row>
-    <row r="143" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="143" spans="6:24">
       <c r="F143" s="7"/>
       <c r="G143" s="7"/>
       <c r="H143" s="7"/>
       <c r="I143" s="19"/>
       <c r="J143" s="19"/>
     </row>
-    <row r="144" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="144" spans="6:24">
       <c r="F144" s="7"/>
       <c r="G144" s="7"/>
       <c r="H144" s="7"/>
       <c r="I144" s="19"/>
       <c r="J144" s="19"/>
     </row>
-    <row r="145" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="145" spans="5:13">
       <c r="F145" s="7"/>
       <c r="G145" s="7"/>
       <c r="H145" s="7"/>
       <c r="I145" s="19"/>
       <c r="J145" s="19"/>
     </row>
-    <row r="146" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="146" spans="5:13">
       <c r="F146" s="7"/>
       <c r="G146" s="7"/>
       <c r="H146" s="7"/>
       <c r="I146" s="19"/>
       <c r="J146" s="19"/>
     </row>
-    <row r="147" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="147" spans="5:13">
       <c r="F147" s="7"/>
       <c r="G147" s="7"/>
       <c r="H147" s="7"/>
       <c r="I147" s="19"/>
       <c r="J147" s="19"/>
     </row>
-    <row r="148" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="148" spans="5:13">
       <c r="F148" s="7"/>
       <c r="G148" s="7"/>
       <c r="H148" s="7"/>
       <c r="I148" s="19"/>
       <c r="J148" s="19"/>
     </row>
-    <row r="149" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="149" spans="5:13">
       <c r="F149" s="7"/>
       <c r="G149" s="7"/>
       <c r="H149" s="7"/>
       <c r="I149" s="19"/>
       <c r="J149" s="19"/>
     </row>
-    <row r="150" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="150" spans="5:13">
       <c r="F150" s="7"/>
       <c r="G150" s="7"/>
       <c r="H150" s="7"/>
       <c r="I150" s="19"/>
       <c r="J150" s="19"/>
     </row>
-    <row r="151" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="151" spans="5:13">
       <c r="F151" s="7"/>
       <c r="G151" s="7"/>
       <c r="H151" s="7"/>
       <c r="I151" s="19"/>
       <c r="J151" s="19"/>
     </row>
-    <row r="152" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="152" spans="5:13">
       <c r="F152" s="7"/>
       <c r="G152" s="7"/>
       <c r="H152" s="7"/>
       <c r="I152" s="19"/>
       <c r="J152" s="19"/>
     </row>
-    <row r="153" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="153" spans="5:13">
       <c r="F153" s="7"/>
       <c r="G153" s="7"/>
       <c r="H153" s="7"/>
       <c r="I153" s="19"/>
       <c r="J153" s="19"/>
     </row>
-    <row r="154" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="154" spans="5:13">
       <c r="F154" s="7"/>
       <c r="G154" s="7"/>
       <c r="H154" s="7"/>
       <c r="I154" s="19"/>
       <c r="J154" s="19"/>
     </row>
-    <row r="155" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="155" spans="5:13">
       <c r="F155" s="150"/>
       <c r="G155" s="150"/>
       <c r="H155" s="7"/>
@@ -10442,7 +10415,7 @@
       <c r="L155" s="43"/>
       <c r="M155" s="5"/>
     </row>
-    <row r="156" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="156" spans="5:13">
       <c r="E156" s="7"/>
       <c r="F156" s="7"/>
       <c r="G156" s="7"/>
@@ -10450,7 +10423,7 @@
       <c r="I156" s="19"/>
       <c r="J156" s="19"/>
     </row>
-    <row r="157" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="157" spans="5:13">
       <c r="E157" s="7"/>
       <c r="F157" s="7"/>
       <c r="G157" s="7"/>
@@ -10458,7 +10431,7 @@
       <c r="I157" s="19"/>
       <c r="J157" s="19"/>
     </row>
-    <row r="158" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="158" spans="5:13">
       <c r="E158" s="7"/>
       <c r="F158" s="7"/>
       <c r="G158" s="7"/>
@@ -10466,7 +10439,7 @@
       <c r="I158" s="19"/>
       <c r="J158" s="19"/>
     </row>
-    <row r="159" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="159" spans="5:13">
       <c r="E159" s="7"/>
       <c r="F159" s="7"/>
       <c r="G159" s="7"/>
@@ -10474,7 +10447,7 @@
       <c r="I159" s="19"/>
       <c r="J159" s="19"/>
     </row>
-    <row r="160" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="160" spans="5:13">
       <c r="E160" s="7"/>
       <c r="F160" s="7"/>
       <c r="G160" s="7"/>
@@ -10482,7 +10455,7 @@
       <c r="I160" s="19"/>
       <c r="J160" s="19"/>
     </row>
-    <row r="161" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="161" spans="5:10">
       <c r="E161" s="7"/>
       <c r="F161" s="7"/>
       <c r="G161" s="7"/>
@@ -10490,7 +10463,7 @@
       <c r="I161" s="19"/>
       <c r="J161" s="19"/>
     </row>
-    <row r="162" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="162" spans="5:10">
       <c r="E162" s="7"/>
       <c r="F162" s="7"/>
       <c r="G162" s="7"/>
@@ -10498,7 +10471,7 @@
       <c r="I162" s="19"/>
       <c r="J162" s="19"/>
     </row>
-    <row r="163" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="163" spans="5:10">
       <c r="E163" s="7"/>
       <c r="F163" s="7"/>
       <c r="G163" s="7"/>
@@ -10506,7 +10479,7 @@
       <c r="I163" s="19"/>
       <c r="J163" s="19"/>
     </row>
-    <row r="164" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="164" spans="5:10">
       <c r="E164" s="7"/>
       <c r="F164" s="7"/>
       <c r="G164" s="7"/>
@@ -10514,7 +10487,7 @@
       <c r="I164" s="19"/>
       <c r="J164" s="19"/>
     </row>
-    <row r="165" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="165" spans="5:10">
       <c r="E165" s="7"/>
       <c r="F165" s="7"/>
       <c r="G165" s="7"/>
@@ -10522,7 +10495,7 @@
       <c r="I165" s="19"/>
       <c r="J165" s="19"/>
     </row>
-    <row r="166" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="166" spans="5:10">
       <c r="E166" s="7"/>
       <c r="F166" s="7"/>
       <c r="G166" s="7"/>
@@ -10530,7 +10503,7 @@
       <c r="I166" s="19"/>
       <c r="J166" s="19"/>
     </row>
-    <row r="167" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="167" spans="5:10">
       <c r="E167" s="7"/>
       <c r="F167" s="7"/>
       <c r="G167" s="7"/>
@@ -10538,7 +10511,7 @@
       <c r="I167" s="19"/>
       <c r="J167" s="19"/>
     </row>
-    <row r="168" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="168" spans="5:10">
       <c r="E168" s="7"/>
       <c r="F168" s="7"/>
       <c r="G168" s="7"/>
@@ -10546,7 +10519,7 @@
       <c r="I168" s="19"/>
       <c r="J168" s="19"/>
     </row>
-    <row r="169" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="169" spans="5:10">
       <c r="E169" s="7"/>
       <c r="F169" s="7"/>
       <c r="G169" s="7"/>
@@ -10554,7 +10527,7 @@
       <c r="I169" s="19"/>
       <c r="J169" s="19"/>
     </row>
-    <row r="170" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="170" spans="5:10">
       <c r="E170" s="7"/>
       <c r="F170" s="7"/>
       <c r="G170" s="7"/>
@@ -10562,7 +10535,7 @@
       <c r="I170" s="19"/>
       <c r="J170" s="19"/>
     </row>
-    <row r="171" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="171" spans="5:10">
       <c r="E171" s="7"/>
       <c r="F171" s="7"/>
       <c r="G171" s="7"/>
@@ -10570,7 +10543,7 @@
       <c r="I171" s="19"/>
       <c r="J171" s="19"/>
     </row>
-    <row r="172" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="172" spans="5:10">
       <c r="E172" s="7"/>
       <c r="F172" s="7"/>
       <c r="G172" s="7"/>
@@ -10578,7 +10551,7 @@
       <c r="I172" s="19"/>
       <c r="J172" s="19"/>
     </row>
-    <row r="173" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="173" spans="5:10">
       <c r="E173" s="7"/>
       <c r="F173" s="7"/>
       <c r="G173" s="7"/>
@@ -10586,7 +10559,7 @@
       <c r="I173" s="19"/>
       <c r="J173" s="19"/>
     </row>
-    <row r="174" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="174" spans="5:10">
       <c r="E174" s="7"/>
       <c r="F174" s="7"/>
       <c r="G174" s="7"/>
@@ -10594,7 +10567,7 @@
       <c r="I174" s="19"/>
       <c r="J174" s="19"/>
     </row>
-    <row r="175" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="175" spans="5:10">
       <c r="E175" s="7"/>
       <c r="F175" s="7"/>
       <c r="G175" s="7"/>
@@ -10602,7 +10575,7 @@
       <c r="I175" s="19"/>
       <c r="J175" s="19"/>
     </row>
-    <row r="176" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="176" spans="5:10">
       <c r="E176" s="7"/>
       <c r="F176" s="7"/>
       <c r="G176" s="7"/>
@@ -10610,7 +10583,7 @@
       <c r="I176" s="19"/>
       <c r="J176" s="19"/>
     </row>
-    <row r="177" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="177" spans="5:10">
       <c r="E177" s="7"/>
       <c r="F177" s="7"/>
       <c r="G177" s="7"/>
@@ -10618,7 +10591,7 @@
       <c r="I177" s="19"/>
       <c r="J177" s="19"/>
     </row>
-    <row r="178" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="178" spans="5:10">
       <c r="E178" s="7"/>
       <c r="F178" s="7"/>
       <c r="G178" s="7"/>
@@ -10626,7 +10599,7 @@
       <c r="I178" s="19"/>
       <c r="J178" s="19"/>
     </row>
-    <row r="179" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="179" spans="5:10">
       <c r="E179" s="7"/>
       <c r="F179" s="7"/>
       <c r="G179" s="7"/>
@@ -10634,7 +10607,7 @@
       <c r="I179" s="19"/>
       <c r="J179" s="19"/>
     </row>
-    <row r="180" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="180" spans="5:10">
       <c r="E180" s="7"/>
       <c r="F180" s="7"/>
       <c r="G180" s="7"/>
@@ -10642,7 +10615,7 @@
       <c r="I180" s="19"/>
       <c r="J180" s="19"/>
     </row>
-    <row r="181" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="181" spans="5:10">
       <c r="E181" s="7"/>
       <c r="F181" s="7"/>
       <c r="G181" s="7"/>
@@ -10650,7 +10623,7 @@
       <c r="I181" s="19"/>
       <c r="J181" s="19"/>
     </row>
-    <row r="182" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="182" spans="5:10">
       <c r="E182" s="7"/>
       <c r="F182" s="7"/>
       <c r="G182" s="7"/>
@@ -10658,7 +10631,7 @@
       <c r="I182" s="19"/>
       <c r="J182" s="19"/>
     </row>
-    <row r="183" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="183" spans="5:10">
       <c r="E183" s="7"/>
       <c r="F183" s="7"/>
       <c r="G183" s="7"/>
@@ -10666,7 +10639,7 @@
       <c r="I183" s="19"/>
       <c r="J183" s="19"/>
     </row>
-    <row r="184" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="184" spans="5:10">
       <c r="E184" s="7"/>
       <c r="F184" s="7"/>
       <c r="G184" s="7"/>
@@ -10674,7 +10647,7 @@
       <c r="I184" s="19"/>
       <c r="J184" s="19"/>
     </row>
-    <row r="185" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="185" spans="5:10">
       <c r="E185" s="7"/>
       <c r="F185" s="7"/>
       <c r="G185" s="7"/>
@@ -10682,7 +10655,7 @@
       <c r="I185" s="19"/>
       <c r="J185" s="19"/>
     </row>
-    <row r="186" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="186" spans="5:10">
       <c r="E186" s="7"/>
       <c r="F186" s="7"/>
       <c r="G186" s="7"/>
@@ -10690,7 +10663,7 @@
       <c r="I186" s="19"/>
       <c r="J186" s="19"/>
     </row>
-    <row r="187" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="187" spans="5:10">
       <c r="E187" s="7"/>
       <c r="F187" s="7"/>
       <c r="G187" s="7"/>
@@ -10698,7 +10671,7 @@
       <c r="I187" s="19"/>
       <c r="J187" s="19"/>
     </row>
-    <row r="188" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="188" spans="5:10">
       <c r="E188" s="7"/>
       <c r="F188" s="7"/>
       <c r="G188" s="7"/>
@@ -10706,7 +10679,7 @@
       <c r="I188" s="19"/>
       <c r="J188" s="19"/>
     </row>
-    <row r="189" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="189" spans="5:10">
       <c r="E189" s="7"/>
       <c r="F189" s="7"/>
       <c r="G189" s="7"/>
@@ -10714,7 +10687,7 @@
       <c r="I189" s="19"/>
       <c r="J189" s="19"/>
     </row>
-    <row r="190" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="190" spans="5:10">
       <c r="E190" s="7"/>
       <c r="F190" s="7"/>
       <c r="G190" s="7"/>
@@ -10722,7 +10695,7 @@
       <c r="I190" s="19"/>
       <c r="J190" s="19"/>
     </row>
-    <row r="191" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="191" spans="5:10">
       <c r="E191" s="7"/>
       <c r="F191" s="7"/>
       <c r="G191" s="7"/>
@@ -10730,7 +10703,7 @@
       <c r="I191" s="19"/>
       <c r="J191" s="19"/>
     </row>
-    <row r="192" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="192" spans="5:10">
       <c r="E192" s="7"/>
       <c r="F192" s="7"/>
       <c r="G192" s="7"/>
@@ -10738,7 +10711,7 @@
       <c r="I192" s="19"/>
       <c r="J192" s="19"/>
     </row>
-    <row r="193" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="193" spans="5:10">
       <c r="E193" s="7"/>
       <c r="F193" s="7"/>
       <c r="G193" s="7"/>
@@ -10746,7 +10719,7 @@
       <c r="I193" s="19"/>
       <c r="J193" s="19"/>
     </row>
-    <row r="194" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="194" spans="5:10">
       <c r="E194" s="7"/>
       <c r="F194" s="7"/>
       <c r="G194" s="7"/>
@@ -10754,7 +10727,7 @@
       <c r="I194" s="19"/>
       <c r="J194" s="19"/>
     </row>
-    <row r="195" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="195" spans="5:10">
       <c r="E195" s="7"/>
       <c r="F195" s="7"/>
       <c r="G195" s="7"/>
@@ -10762,7 +10735,7 @@
       <c r="I195" s="19"/>
       <c r="J195" s="19"/>
     </row>
-    <row r="196" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="196" spans="5:10">
       <c r="E196" s="7"/>
       <c r="F196" s="7"/>
       <c r="G196" s="7"/>
@@ -10770,7 +10743,7 @@
       <c r="I196" s="19"/>
       <c r="J196" s="19"/>
     </row>
-    <row r="197" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="197" spans="5:10">
       <c r="E197" s="7"/>
       <c r="F197" s="7"/>
       <c r="G197" s="7"/>
@@ -10778,7 +10751,7 @@
       <c r="I197" s="19"/>
       <c r="J197" s="19"/>
     </row>
-    <row r="198" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="198" spans="5:10">
       <c r="E198" s="7"/>
       <c r="F198" s="7"/>
       <c r="G198" s="7"/>
@@ -10786,7 +10759,7 @@
       <c r="I198" s="19"/>
       <c r="J198" s="19"/>
     </row>
-    <row r="199" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="199" spans="5:10">
       <c r="E199" s="7"/>
       <c r="F199" s="7"/>
       <c r="G199" s="7"/>
@@ -10794,7 +10767,7 @@
       <c r="I199" s="19"/>
       <c r="J199" s="19"/>
     </row>
-    <row r="200" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="200" spans="5:10">
       <c r="E200" s="7"/>
       <c r="F200" s="7"/>
       <c r="G200" s="7"/>
@@ -10802,7 +10775,7 @@
       <c r="I200" s="19"/>
       <c r="J200" s="19"/>
     </row>
-    <row r="201" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="201" spans="5:10">
       <c r="E201" s="7"/>
       <c r="F201" s="7"/>
       <c r="G201" s="7"/>
@@ -10810,7 +10783,7 @@
       <c r="I201" s="19"/>
       <c r="J201" s="19"/>
     </row>
-    <row r="202" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="202" spans="5:10">
       <c r="E202" s="7"/>
       <c r="F202" s="7"/>
       <c r="G202" s="7"/>
@@ -10818,7 +10791,7 @@
       <c r="I202" s="19"/>
       <c r="J202" s="19"/>
     </row>
-    <row r="203" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="203" spans="5:10">
       <c r="E203" s="7"/>
       <c r="F203" s="7"/>
       <c r="G203" s="7"/>
@@ -10826,7 +10799,7 @@
       <c r="I203" s="19"/>
       <c r="J203" s="19"/>
     </row>
-    <row r="204" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="204" spans="5:10">
       <c r="E204" s="7"/>
       <c r="F204" s="7"/>
       <c r="G204" s="7"/>
@@ -10834,7 +10807,7 @@
       <c r="I204" s="19"/>
       <c r="J204" s="19"/>
     </row>
-    <row r="205" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="205" spans="5:10">
       <c r="E205" s="7"/>
       <c r="F205" s="7"/>
       <c r="G205" s="7"/>
@@ -10842,7 +10815,7 @@
       <c r="I205" s="19"/>
       <c r="J205" s="19"/>
     </row>
-    <row r="206" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="206" spans="5:10">
       <c r="E206" s="7"/>
       <c r="F206" s="7"/>
       <c r="G206" s="7"/>
@@ -10850,7 +10823,7 @@
       <c r="I206" s="19"/>
       <c r="J206" s="19"/>
     </row>
-    <row r="207" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="207" spans="5:10">
       <c r="E207" s="7"/>
       <c r="F207" s="7"/>
       <c r="G207" s="7"/>
@@ -10858,7 +10831,7 @@
       <c r="I207" s="19"/>
       <c r="J207" s="19"/>
     </row>
-    <row r="208" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="208" spans="5:10">
       <c r="E208" s="7"/>
       <c r="F208" s="7"/>
       <c r="G208" s="7"/>
@@ -10866,7 +10839,7 @@
       <c r="I208" s="19"/>
       <c r="J208" s="19"/>
     </row>
-    <row r="209" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="209" spans="5:10">
       <c r="E209" s="7"/>
       <c r="F209" s="7"/>
       <c r="G209" s="7"/>
@@ -10874,7 +10847,7 @@
       <c r="I209" s="19"/>
       <c r="J209" s="19"/>
     </row>
-    <row r="210" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="210" spans="5:10">
       <c r="E210" s="7"/>
       <c r="F210" s="7"/>
       <c r="G210" s="7"/>
@@ -10882,7 +10855,7 @@
       <c r="I210" s="19"/>
       <c r="J210" s="19"/>
     </row>
-    <row r="211" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="211" spans="5:10">
       <c r="E211" s="7"/>
       <c r="F211" s="7"/>
       <c r="G211" s="7"/>
@@ -10890,7 +10863,7 @@
       <c r="I211" s="19"/>
       <c r="J211" s="19"/>
     </row>
-    <row r="212" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="212" spans="5:10">
       <c r="E212" s="7"/>
       <c r="F212" s="7"/>
       <c r="G212" s="7"/>
@@ -10898,7 +10871,7 @@
       <c r="I212" s="19"/>
       <c r="J212" s="19"/>
     </row>
-    <row r="213" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="213" spans="5:10">
       <c r="E213" s="7"/>
       <c r="F213" s="7"/>
       <c r="G213" s="7"/>
@@ -10906,7 +10879,7 @@
       <c r="I213" s="19"/>
       <c r="J213" s="19"/>
     </row>
-    <row r="214" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="214" spans="5:10">
       <c r="E214" s="7"/>
       <c r="F214" s="7"/>
       <c r="G214" s="7"/>
@@ -10914,7 +10887,7 @@
       <c r="I214" s="19"/>
       <c r="J214" s="19"/>
     </row>
-    <row r="215" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="215" spans="5:10">
       <c r="E215" s="7"/>
       <c r="F215" s="7"/>
       <c r="G215" s="7"/>
@@ -10922,7 +10895,7 @@
       <c r="I215" s="19"/>
       <c r="J215" s="19"/>
     </row>
-    <row r="216" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="216" spans="5:10">
       <c r="E216" s="7"/>
       <c r="F216" s="7"/>
       <c r="G216" s="7"/>
@@ -10930,7 +10903,7 @@
       <c r="I216" s="19"/>
       <c r="J216" s="19"/>
     </row>
-    <row r="217" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="217" spans="5:10">
       <c r="E217" s="7"/>
       <c r="F217" s="7"/>
       <c r="G217" s="7"/>
@@ -10938,7 +10911,7 @@
       <c r="I217" s="19"/>
       <c r="J217" s="19"/>
     </row>
-    <row r="218" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="218" spans="5:10">
       <c r="E218" s="7"/>
       <c r="F218" s="7"/>
       <c r="G218" s="7"/>
@@ -10946,7 +10919,7 @@
       <c r="I218" s="19"/>
       <c r="J218" s="19"/>
     </row>
-    <row r="219" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="219" spans="5:10">
       <c r="E219" s="7"/>
       <c r="F219" s="7"/>
       <c r="G219" s="7"/>
@@ -10954,7 +10927,7 @@
       <c r="I219" s="19"/>
       <c r="J219" s="19"/>
     </row>
-    <row r="220" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="220" spans="5:10">
       <c r="E220" s="7"/>
       <c r="F220" s="7"/>
       <c r="G220" s="7"/>
@@ -10962,7 +10935,7 @@
       <c r="I220" s="19"/>
       <c r="J220" s="19"/>
     </row>
-    <row r="221" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="221" spans="5:10">
       <c r="E221" s="7"/>
       <c r="F221" s="7"/>
       <c r="G221" s="7"/>
@@ -10970,7 +10943,7 @@
       <c r="I221" s="19"/>
       <c r="J221" s="19"/>
     </row>
-    <row r="222" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="222" spans="5:10">
       <c r="E222" s="7"/>
       <c r="F222" s="7"/>
       <c r="G222" s="7"/>
@@ -10978,7 +10951,7 @@
       <c r="I222" s="19"/>
       <c r="J222" s="19"/>
     </row>
-    <row r="223" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="223" spans="5:10">
       <c r="E223" s="7"/>
       <c r="F223" s="7"/>
       <c r="G223" s="7"/>
@@ -10986,7 +10959,7 @@
       <c r="I223" s="19"/>
       <c r="J223" s="19"/>
     </row>
-    <row r="224" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="224" spans="5:10">
       <c r="E224" s="7"/>
       <c r="F224" s="7"/>
       <c r="G224" s="7"/>
@@ -10994,7 +10967,7 @@
       <c r="I224" s="19"/>
       <c r="J224" s="19"/>
     </row>
-    <row r="225" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="225" spans="5:10">
       <c r="E225" s="7"/>
       <c r="F225" s="7"/>
       <c r="G225" s="7"/>
@@ -11002,7 +10975,7 @@
       <c r="I225" s="19"/>
       <c r="J225" s="19"/>
     </row>
-    <row r="226" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="226" spans="5:10">
       <c r="E226" s="7"/>
       <c r="F226" s="7"/>
       <c r="G226" s="7"/>
@@ -11010,7 +10983,7 @@
       <c r="I226" s="19"/>
       <c r="J226" s="19"/>
     </row>
-    <row r="227" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="227" spans="5:10">
       <c r="E227" s="7"/>
       <c r="F227" s="7"/>
       <c r="G227" s="7"/>
@@ -11018,7 +10991,7 @@
       <c r="I227" s="19"/>
       <c r="J227" s="19"/>
     </row>
-    <row r="228" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="228" spans="5:10">
       <c r="E228" s="7"/>
       <c r="F228" s="7"/>
       <c r="G228" s="7"/>
@@ -11026,7 +10999,7 @@
       <c r="I228" s="19"/>
       <c r="J228" s="19"/>
     </row>
-    <row r="229" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="229" spans="5:10">
       <c r="E229" s="7"/>
       <c r="F229" s="7"/>
       <c r="G229" s="7"/>
@@ -11034,7 +11007,7 @@
       <c r="I229" s="19"/>
       <c r="J229" s="19"/>
     </row>
-    <row r="230" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="230" spans="5:10">
       <c r="E230" s="7"/>
       <c r="F230" s="7"/>
       <c r="G230" s="7"/>
@@ -11042,7 +11015,7 @@
       <c r="I230" s="19"/>
       <c r="J230" s="19"/>
     </row>
-    <row r="231" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="231" spans="5:10">
       <c r="E231" s="7"/>
       <c r="F231" s="7"/>
       <c r="G231" s="7"/>

</xml_diff>